<commit_message>
Fixed bug in altCount causing interval to drop to 0, leading to timer endless loop
</commit_message>
<xml_diff>
--- a/flora_blink_button/Notes on sweep.xlsx
+++ b/flora_blink_button/Notes on sweep.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6888" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>int nextLine = prevLine + sweepDir;</t>
   </si>
@@ -78,6 +79,21 @@
   </si>
   <si>
     <t>first round</t>
+  </si>
+  <si>
+    <t>cycleCount</t>
+  </si>
+  <si>
+    <t>altCount</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>Don't modify interval at beginning of round 0</t>
+  </si>
+  <si>
+    <t>timeDir</t>
   </si>
 </sst>
 </file>
@@ -404,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -595,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C17" si="5">A8+B8</f>
+        <f t="shared" ref="C8:C15" si="5">A8+B8</f>
         <v>4</v>
       </c>
       <c r="E8">
@@ -1076,4 +1092,413 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.3671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>C2+(D2*100)</f>
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C9" si="0">C3+(D3*100)</f>
+        <v>400</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C26" si="1">C9+(D9*100)</f>
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>